<commit_message>
better randomness of numbers for benchmark
</commit_message>
<xml_diff>
--- a/02-algorithms/03-algorithms-sorting/bar_chart.xlsx
+++ b/02-algorithms/03-algorithms-sorting/bar_chart.xlsx
@@ -8,21 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lcaton/bloc/sep-assignments/02-algorithms/03-sorting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A1263D-A762-0549-BA80-8C4AD38E1716}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C0A1602-560F-FE4C-A364-FD91340715C5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28140" yWindow="4540" windowWidth="27640" windowHeight="16940" xr2:uid="{2E6420F0-202A-EA4E-B2FA-A789BA8665F9}"/>
+    <workbookView xWindow="1320" yWindow="2160" windowWidth="27640" windowHeight="16940" xr2:uid="{2E6420F0-202A-EA4E-B2FA-A789BA8665F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$6:$A$8</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$2:$B$5</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$6:$B$8</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$A$6:$A$8</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$B$2:$B$5</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$B$6:$B$8</definedName>
-  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -245,25 +237,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>7.4999999999999993E-5</c:v>
+                  <c:v>1.7899999999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.5000000000000003E-5</c:v>
+                  <c:v>4.0099999999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.0000000000000004E-6</c:v>
+                  <c:v>6.0000000000000002E-6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.9999999999999996E-6</c:v>
+                  <c:v>1.1E-5</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>5.0000000000000004E-6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.9999999999999998E-6</c:v>
+                  <c:v>7.9999999999999996E-6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.6E-5</c:v>
+                  <c:v>1.4E-5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1323,7 +1315,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{489F68E2-0A13-2942-A558-446AAFE7BC5F}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1344,7 +1338,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3">
-        <v>7.4999999999999993E-5</v>
+        <v>1.7899999999999999E-4</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="19" x14ac:dyDescent="0.25">
@@ -1352,7 +1346,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3">
-        <v>4.5000000000000003E-5</v>
+        <v>4.0099999999999999E-4</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="19" x14ac:dyDescent="0.25">
@@ -1360,7 +1354,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3">
-        <v>5.0000000000000004E-6</v>
+        <v>6.0000000000000002E-6</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="19" x14ac:dyDescent="0.25">
@@ -1368,7 +1362,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="3">
-        <v>7.9999999999999996E-6</v>
+        <v>1.1E-5</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="19" x14ac:dyDescent="0.25">
@@ -1384,7 +1378,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="3">
-        <v>3.9999999999999998E-6</v>
+        <v>7.9999999999999996E-6</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="19" x14ac:dyDescent="0.25">
@@ -1392,7 +1386,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="3">
-        <v>4.6E-5</v>
+        <v>1.4E-5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>